<commit_message>
pan card verification added
</commit_message>
<xml_diff>
--- a/Datasets/PanCard.xlsx
+++ b/Datasets/PanCard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rohan_Folders\Education\BTech_Engineering\16th Standard_TSEC_4th Year(BE)\Semester VIII\TSEC\Major Project(PR)\Semester-VIII\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malan\Documents\GitHub\Document-Verification-OCR\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EBB518-982E-458A-B12E-F133AE2AAE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459973D7-CA9D-4600-9C13-EFCDC6A8D960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -648,7 +648,7 @@
     <t>AEFFD7587L</t>
   </si>
   <si>
-    <t>17/07/1986</t>
+    <t>16/07/1986</t>
   </si>
 </sst>
 </file>
@@ -981,18 +981,18 @@
   <dimension ref="A1:D102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1015,7 +1015,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>64257</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>46998</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>42403</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>21824</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>49773</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>51594</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>11785</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>19608</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>65540</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>54102</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>31837</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>10397</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>9557</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>3745</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>58506</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>59049</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>54863</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>39</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>6379</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>72930</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>27062</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>45</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>50066</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>47</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>53420</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>49</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>3168</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>51</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>71409</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>53</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>27125</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>55</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>11489</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>63844</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>59</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>15038</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>61</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>69825</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>63</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>65</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>10799</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>67</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>35861</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>69</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>27823</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>71</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>72322</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>73</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>2594</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>75</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>70725</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>77</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>26669</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>79</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>54902</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>81</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>59390</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>83</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>29757</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>85</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>20182</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>87</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>57841</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>89</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>65962</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>91</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>7827</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>93</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>32203</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>95</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>65419</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>97</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>52359</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>99</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>39486</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>101</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>56618</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>103</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>60791</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>105</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>11728</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>107</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>109</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>22463</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>111</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>1559</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>113</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>28350</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>115</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>27768</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>117</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>69587</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>119</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>59934</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>121</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>11874</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>123</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>66239</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>125</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>40306</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>127</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>46603</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>129</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>26854</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>131</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>134</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>67812</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>136</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>40503</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>138</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>42103</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>140</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>10844</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>142</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>68409</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>144</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>69401</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>146</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>68677</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>148</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>36540</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>150</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>49010</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>152</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>11829</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>154</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>156</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>8561</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>158</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>34034</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>160</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>63071</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>162</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>63434</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>164</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>63640</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>166</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>22757</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>168</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>12426</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>170</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>34390</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>172</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>64985</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>174</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>12150</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>176</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>8653</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>178</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>24164</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>180</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>4400</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>182</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>53729</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>184</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>16837</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>186</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>65782</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>188</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>54457</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>190</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>26315</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>192</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>195</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>22404</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>197</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>64713</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>199</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>54976</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>201</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>4081</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>203</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>55765</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>205</v>
       </c>

</xml_diff>